<commit_message>
create Session for client and save in database
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nodejs\who-is-undercover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46A462A-1137-47CC-9B60-28FEAAD7F6AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A365580-C71E-4DFA-A38E-43D3BE3E8588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="212">
   <si>
     <t>初恋</t>
   </si>
@@ -592,6 +592,75 @@
   </si>
   <si>
     <t>COVID-19</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>甄子丹</t>
+  </si>
+  <si>
+    <t>李连杰</t>
+  </si>
+  <si>
+    <t>狼</t>
+  </si>
+  <si>
+    <t>狐狸</t>
+  </si>
+  <si>
+    <t>成龙</t>
+  </si>
+  <si>
+    <t>郭靖</t>
+  </si>
+  <si>
+    <t>杨过</t>
+  </si>
+  <si>
+    <t>红孩儿</t>
+  </si>
+  <si>
+    <t>哪吒</t>
+  </si>
+  <si>
+    <t>Punggol</t>
+  </si>
+  <si>
+    <t>Seng Kang</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>NUS</t>
+  </si>
+  <si>
+    <t>Buger King</t>
+  </si>
+  <si>
+    <t>Badminton</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
+  <si>
+    <t>McDonalds</t>
+  </si>
+  <si>
+    <t>白骨精</t>
+  </si>
+  <si>
+    <t>Winnie the Pooh</t>
+  </si>
+  <si>
+    <t>Piglet</t>
+  </si>
+  <si>
+    <t>樱木花道</t>
+  </si>
+  <si>
+    <t>流川枫</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0585F02-79B5-466B-B275-8B18A2A6C1C4}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="J109" sqref="J109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,7 +1056,7 @@
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -997,8 +1066,11 @@
       <c r="C1" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1008,8 +1080,11 @@
       <c r="C2" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1020,7 +1095,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1031,7 +1106,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1042,7 +1117,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1053,7 +1128,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1064,7 +1139,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -1075,7 +1150,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1086,7 +1161,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -1097,7 +1172,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -1108,7 +1183,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1119,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -1130,7 +1205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -1141,7 +1216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -1152,7 +1227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -2065,13 +2140,145 @@
         <v>187</v>
       </c>
     </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1">
+        <v>99</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="1">
+        <v>100</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>101</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>102</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="1">
+        <v>103</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>105</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="1">
+        <v>106</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>107</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>108</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>109</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>110</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C127">
-    <sortCondition ref="A1:A127"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C125">
+    <sortCondition ref="A1:A125"/>
   </sortState>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add language property to Card in db
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nodejs\who-is-undercover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A365580-C71E-4DFA-A38E-43D3BE3E8588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EC80B4-D4DE-40C7-81BD-5A1459BF6A2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="chinese" sheetId="2" r:id="rId1"/>
+    <sheet name="english" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="211">
   <si>
     <t>初恋</t>
   </si>
@@ -592,9 +593,6 @@
   </si>
   <si>
     <t>COVID-19</t>
-  </si>
-  <si>
-    <t>english</t>
   </si>
   <si>
     <t>甄子丹</t>
@@ -714,7 +712,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1045,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0585F02-79B5-466B-B275-8B18A2A6C1C4}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="J109" sqref="J109"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1056,186 +1074,180 @@
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1243,65 +1255,65 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>144</v>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>145</v>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>146</v>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>148</v>
+      <c r="B21" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>150</v>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1309,10 +1321,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1320,10 +1332,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1331,10 +1343,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1342,10 +1354,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1353,10 +1365,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1364,10 +1376,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1375,10 +1387,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1386,10 +1398,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1397,10 +1409,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1408,10 +1420,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1419,10 +1431,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1430,7 +1442,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>24</v>
@@ -1441,10 +1453,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1452,10 +1464,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1463,10 +1475,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1474,10 +1486,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1485,10 +1497,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1496,10 +1508,10 @@
         <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1507,10 +1519,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1518,10 +1530,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1529,65 +1541,65 @@
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>153</v>
+        <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>44</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>128</v>
+      <c r="B44" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>154</v>
+      <c r="B45" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>46</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>156</v>
+      <c r="B46" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>47</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>101</v>
+      <c r="B47" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>48</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>1</v>
+      <c r="B48" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>0</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1595,10 +1607,10 @@
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>160</v>
+        <v>84</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1606,10 +1618,10 @@
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1617,10 +1629,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1628,10 +1640,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1639,10 +1651,10 @@
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1650,10 +1662,10 @@
         <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1661,10 +1673,10 @@
         <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1672,10 +1684,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1683,10 +1695,10 @@
         <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1694,10 +1706,10 @@
         <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1705,10 +1717,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1716,10 +1728,10 @@
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1727,10 +1739,10 @@
         <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1738,131 +1750,131 @@
         <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>63</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>108</v>
+      <c r="B63" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>64</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>110</v>
+      <c r="B64" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>65</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>112</v>
+      <c r="B65" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>66</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>114</v>
+      <c r="B66" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>67</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>116</v>
+      <c r="B67" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>68</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>38</v>
+      <c r="B68" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>69</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>166</v>
+      <c r="B69" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>70</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>37</v>
+      <c r="B70" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>71</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>55</v>
+      <c r="B71" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>72</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>53</v>
+      <c r="B72" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>73</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>36</v>
+      <c r="B73" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1870,10 +1882,10 @@
         <v>74</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1881,10 +1893,10 @@
         <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1892,10 +1904,10 @@
         <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1903,10 +1915,10 @@
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1914,10 +1926,10 @@
         <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1925,10 +1937,10 @@
         <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1936,10 +1948,10 @@
         <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1947,10 +1959,10 @@
         <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1958,10 +1970,10 @@
         <v>82</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1969,10 +1981,10 @@
         <v>83</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1980,10 +1992,10 @@
         <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1991,10 +2003,10 @@
         <v>85</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -2002,10 +2014,10 @@
         <v>86</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -2013,10 +2025,10 @@
         <v>87</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>78</v>
+        <v>178</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -2024,10 +2036,10 @@
         <v>88</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -2035,10 +2047,10 @@
         <v>89</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -2046,10 +2058,10 @@
         <v>90</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -2057,10 +2069,10 @@
         <v>91</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -2068,10 +2080,10 @@
         <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -2079,10 +2091,10 @@
         <v>93</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -2090,10 +2102,10 @@
         <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -2101,10 +2113,10 @@
         <v>95</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -2112,10 +2124,10 @@
         <v>96</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -2123,10 +2135,10 @@
         <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2134,149 +2146,165 @@
         <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="1">
-        <v>99</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="1">
-        <v>100</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="1">
-        <v>101</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="1">
-        <v>102</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="1">
-        <v>103</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C103" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:C98 B111:C1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D2669E-5129-48E0-B150-9D1272E8D56D}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1000</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="1">
-        <v>104</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1010</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="1">
-        <v>105</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="1">
-        <v>106</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="1">
-        <v>107</v>
-      </c>
-      <c r="B107" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="1">
-        <v>108</v>
-      </c>
-      <c r="B108" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1011</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="1">
-        <v>109</v>
-      </c>
-      <c r="B109" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="1">
-        <v>110</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>211</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C125">
-    <sortCondition ref="A1:A125"/>
-  </sortState>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="B1:C12">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add Feedback form and Game Rules on first page
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nodejs\who-is-undercover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EC80B4-D4DE-40C7-81BD-5A1459BF6A2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49A2536-EC46-4F65-9552-989302ED7D30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{60E5C61E-3573-4D78-BCF9-06B87FF2C01F}"/>
   </bookViews>
   <sheets>
     <sheet name="chinese" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="233">
   <si>
     <t>初恋</t>
   </si>
@@ -659,6 +659,72 @@
   </si>
   <si>
     <t>流川枫</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Biden</t>
+  </si>
+  <si>
+    <t>toothbrush</t>
+  </si>
+  <si>
+    <t>toothpaste</t>
+  </si>
+  <si>
+    <t>eyebrow</t>
+  </si>
+  <si>
+    <t>eyelash</t>
+  </si>
+  <si>
+    <t>Spiderman</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>Cinderella</t>
+  </si>
+  <si>
+    <t>Ugly Duckling</t>
+  </si>
+  <si>
+    <t>lip balm</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>lipstick</t>
+  </si>
+  <si>
+    <t>tissue paper</t>
+  </si>
+  <si>
+    <t>handkerchief</t>
+  </si>
+  <si>
+    <t>chilli</t>
+  </si>
+  <si>
+    <t>wasabi</t>
+  </si>
+  <si>
+    <t>security guard</t>
+  </si>
+  <si>
+    <t>bodyguard</t>
+  </si>
+  <si>
+    <t>mirror</t>
+  </si>
+  <si>
+    <t>glass</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0585F02-79B5-466B-B275-8B18A2A6C1C4}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2163,17 +2229,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D2669E-5129-48E0-B150-9D1272E8D56D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>118</v>
@@ -2184,7 +2254,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>120</v>
@@ -2195,7 +2265,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>123</v>
@@ -2206,7 +2276,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>124</v>
@@ -2217,7 +2287,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>148</v>
@@ -2228,7 +2298,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>37</v>
@@ -2239,7 +2309,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>60</v>
@@ -2250,7 +2320,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>205</v>
@@ -2261,7 +2331,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>198</v>
@@ -2272,7 +2342,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>201</v>
@@ -2283,7 +2353,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>203</v>
@@ -2294,7 +2364,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>207</v>
@@ -2303,10 +2373,131 @@
         <v>208</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1013</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1014</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1015</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1016</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1017</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1018</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1019</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1020</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1021</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1022</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1023</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:C12">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="B1:C23">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>